<commit_message>
Small update to survey
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKAGAIN/Forms/MASKAGAIN/MASKAGAIN.xlsx
+++ b/app/config/tables/MASKAGAIN/Forms/MASKAGAIN/MASKAGAIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071506E-D4D2-4473-A6CD-55B21F635CB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC6FC1F-DE28-4BEF-AC89-C0F5BD9040A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="230">
   <si>
     <t>setting_name</t>
   </si>
@@ -718,18 +718,6 @@
   </si>
   <si>
     <t>data("ESTADO") != null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data("DATASAI") != null || data("ESTADO") == "1" || data("ESTADO") == "4" || data("ESTADO") == "6" || data("ESTADO") == "8" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">data("ACCEPT") != null || data("RANGROUP") != 2 || data("ESTADO") == "2" || data("ESTADO") == "3" || data("ESTADO") == "6" || data("ESTADO") == "8" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">data("MASC") != null || data("RANGROUP") != 2 || data("ESTADO") == "2" || data("ESTADO") == "3" || data("ESTADO") == "6" || data("ESTADO") == "8" </t>
-  </si>
-  <si>
-    <t>data("DUPLO") != null || data("ESTADO") != "8"</t>
   </si>
   <si>
     <t>Remember to use masks and wash hands</t>
@@ -1260,9 +1248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,9 +1574,6 @@
       <c r="H27" t="s">
         <v>97</v>
       </c>
-      <c r="J27" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="28" spans="2:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -1678,9 +1663,6 @@
       <c r="H37" t="s">
         <v>108</v>
       </c>
-      <c r="J37" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="38" spans="2:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -1721,9 +1703,6 @@
       <c r="H42" t="s">
         <v>110</v>
       </c>
-      <c r="J42" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="43" spans="2:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -1752,9 +1731,6 @@
       <c r="H45" t="s">
         <v>163</v>
       </c>
-      <c r="J45" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="46" spans="2:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -1806,10 +1782,10 @@
         <v>166</v>
       </c>
       <c r="G52" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H52" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>